<commit_message>
lab6 needs a few more variables and its done
</commit_message>
<xml_diff>
--- a/data/lab6_train_data.xlsx
+++ b/data/lab6_train_data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="526">
   <si>
     <t>Image ID</t>
   </si>
@@ -846,9 +846,6 @@
     <t>Kelly-Image01</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Kelly-Image02</t>
   </si>
   <si>
@@ -1545,6 +1542,9 @@
     <t>TestSetImage04</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>TestSetImage05</t>
   </si>
   <si>
@@ -1667,7 +1667,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1724,9 +1724,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -30037,7 +30034,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>277</v>
+        <v>25</v>
       </c>
       <c r="F2" s="7">
         <v>0.0</v>
@@ -30079,7 +30076,7 @@
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B3" s="6">
         <v>0.0</v>
@@ -30133,7 +30130,7 @@
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B4" s="6">
         <v>1.0</v>
@@ -30187,7 +30184,7 @@
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B5" s="6">
         <v>0.0</v>
@@ -30241,7 +30238,7 @@
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B6" s="6">
         <v>0.0</v>
@@ -30295,7 +30292,7 @@
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B7" s="6">
         <v>0.0</v>
@@ -30349,7 +30346,7 @@
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B8" s="6">
         <v>1.0</v>
@@ -30403,7 +30400,7 @@
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B9" s="6">
         <v>1.0</v>
@@ -30457,7 +30454,7 @@
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B10" s="6">
         <v>1.0</v>
@@ -30511,7 +30508,7 @@
     </row>
     <row r="11">
       <c r="A11" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B11" s="6">
         <v>0.0</v>
@@ -30565,7 +30562,7 @@
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B12" s="6">
         <v>0.0</v>
@@ -30619,7 +30616,7 @@
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B13" s="6">
         <v>1.0</v>
@@ -30673,7 +30670,7 @@
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B14" s="6">
         <v>1.0</v>
@@ -30727,7 +30724,7 @@
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B15" s="6">
         <v>0.0</v>
@@ -30781,7 +30778,7 @@
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B16" s="6">
         <v>1.0</v>
@@ -30793,7 +30790,7 @@
         <v>1.0</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>277</v>
+        <v>25</v>
       </c>
       <c r="F16" s="7">
         <v>1.0</v>
@@ -30835,7 +30832,7 @@
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B17" s="6">
         <v>1.0</v>
@@ -30889,7 +30886,7 @@
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B18" s="6">
         <v>1.0</v>
@@ -30901,7 +30898,7 @@
         <v>1.0</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>277</v>
+        <v>25</v>
       </c>
       <c r="F18" s="7">
         <v>0.0</v>
@@ -30943,7 +30940,7 @@
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B19" s="6">
         <v>1.0</v>
@@ -30955,7 +30952,7 @@
         <v>1.0</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>277</v>
+        <v>25</v>
       </c>
       <c r="F19" s="7">
         <v>0.0</v>
@@ -30997,7 +30994,7 @@
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B20" s="6">
         <v>0.0</v>
@@ -31009,7 +31006,7 @@
         <v>1.0</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>277</v>
+        <v>25</v>
       </c>
       <c r="F20" s="7">
         <v>0.0</v>
@@ -31051,7 +31048,7 @@
     </row>
     <row r="21">
       <c r="A21" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B21" s="6">
         <v>1.0</v>
@@ -31105,7 +31102,7 @@
     </row>
     <row r="22">
       <c r="A22" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B22" s="6">
         <v>0.0</v>
@@ -31159,7 +31156,7 @@
     </row>
     <row r="23">
       <c r="A23" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B23" s="6">
         <v>0.0</v>
@@ -31213,7 +31210,7 @@
     </row>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B24" s="6">
         <v>0.0</v>
@@ -31267,7 +31264,7 @@
     </row>
     <row r="25">
       <c r="A25" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B25" s="6">
         <v>0.0</v>
@@ -31321,7 +31318,7 @@
     </row>
     <row r="26">
       <c r="A26" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B26" s="6">
         <v>0.0</v>
@@ -31375,7 +31372,7 @@
     </row>
     <row r="27">
       <c r="A27" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B27" s="6">
         <v>0.0</v>
@@ -31429,7 +31426,7 @@
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B28" s="6">
         <v>0.0</v>
@@ -31483,7 +31480,7 @@
     </row>
     <row r="29">
       <c r="A29" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B29" s="6">
         <v>1.0</v>
@@ -31537,7 +31534,7 @@
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B30" s="6">
         <v>0.0</v>
@@ -31591,7 +31588,7 @@
     </row>
     <row r="31">
       <c r="A31" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B31" s="6">
         <v>0.0</v>
@@ -31645,7 +31642,7 @@
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B32" s="6">
         <v>1.0</v>
@@ -31699,7 +31696,7 @@
     </row>
     <row r="33">
       <c r="A33" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B33" s="6">
         <v>1.0</v>
@@ -31753,7 +31750,7 @@
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B34" s="6">
         <v>1.0</v>
@@ -31807,7 +31804,7 @@
     </row>
     <row r="35">
       <c r="A35" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B35" s="6">
         <v>0.0</v>
@@ -31861,7 +31858,7 @@
     </row>
     <row r="36">
       <c r="A36" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B36" s="6">
         <v>0.0</v>
@@ -31915,7 +31912,7 @@
     </row>
     <row r="37">
       <c r="A37" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B37" s="6">
         <v>0.0</v>
@@ -31969,7 +31966,7 @@
     </row>
     <row r="38">
       <c r="A38" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B38" s="6">
         <v>0.0</v>
@@ -32023,7 +32020,7 @@
     </row>
     <row r="39">
       <c r="A39" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B39" s="6">
         <v>0.0</v>
@@ -32077,7 +32074,7 @@
     </row>
     <row r="40">
       <c r="A40" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B40" s="6">
         <v>0.0</v>
@@ -32131,7 +32128,7 @@
     </row>
     <row r="41">
       <c r="A41" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B41" s="6">
         <v>1.0</v>
@@ -32185,7 +32182,7 @@
     </row>
     <row r="42">
       <c r="A42" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B42" s="6">
         <v>1.0</v>
@@ -32239,7 +32236,7 @@
     </row>
     <row r="43">
       <c r="A43" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B43" s="6">
         <v>0.0</v>
@@ -32293,7 +32290,7 @@
     </row>
     <row r="44">
       <c r="A44" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B44" s="6">
         <v>1.0</v>
@@ -32347,7 +32344,7 @@
     </row>
     <row r="45">
       <c r="A45" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B45" s="6">
         <v>0.0</v>
@@ -32401,7 +32398,7 @@
     </row>
     <row r="46">
       <c r="A46" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B46" s="6">
         <v>1.0</v>
@@ -32455,7 +32452,7 @@
     </row>
     <row r="47">
       <c r="A47" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B47" s="6">
         <v>1.0</v>
@@ -32509,7 +32506,7 @@
     </row>
     <row r="48">
       <c r="A48" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B48" s="6">
         <v>1.0</v>
@@ -32563,7 +32560,7 @@
     </row>
     <row r="49">
       <c r="A49" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B49" s="6">
         <v>0.0</v>
@@ -32617,7 +32614,7 @@
     </row>
     <row r="50">
       <c r="A50" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B50" s="6">
         <v>0.0</v>
@@ -32671,7 +32668,7 @@
     </row>
     <row r="51">
       <c r="A51" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B51" s="6">
         <v>1.0</v>
@@ -32725,7 +32722,7 @@
     </row>
     <row r="52">
       <c r="A52" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B52" s="6">
         <v>0.0</v>
@@ -32779,7 +32776,7 @@
     </row>
     <row r="53">
       <c r="A53" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B53" s="6">
         <v>1.0</v>
@@ -32833,7 +32830,7 @@
     </row>
     <row r="54">
       <c r="A54" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B54" s="6">
         <v>1.0</v>
@@ -32887,7 +32884,7 @@
     </row>
     <row r="55">
       <c r="A55" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B55" s="6">
         <v>1.0</v>
@@ -32941,7 +32938,7 @@
     </row>
     <row r="56">
       <c r="A56" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B56" s="6">
         <v>0.0</v>
@@ -32995,7 +32992,7 @@
     </row>
     <row r="57">
       <c r="A57" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B57" s="6">
         <v>1.0</v>
@@ -33049,7 +33046,7 @@
     </row>
     <row r="58">
       <c r="A58" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B58" s="6">
         <v>0.0</v>
@@ -33103,7 +33100,7 @@
     </row>
     <row r="59">
       <c r="A59" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B59" s="6">
         <v>1.0</v>
@@ -33157,7 +33154,7 @@
     </row>
     <row r="60">
       <c r="A60" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B60" s="6">
         <v>0.0</v>
@@ -33211,7 +33208,7 @@
     </row>
     <row r="61">
       <c r="A61" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B61" s="6">
         <v>0.0</v>
@@ -33265,7 +33262,7 @@
     </row>
     <row r="62">
       <c r="A62" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B62" s="6">
         <v>0.0</v>
@@ -33319,7 +33316,7 @@
     </row>
     <row r="63">
       <c r="A63" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B63" s="6">
         <v>0.0</v>
@@ -33373,7 +33370,7 @@
     </row>
     <row r="64">
       <c r="A64" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B64" s="6">
         <v>0.0</v>
@@ -33427,7 +33424,7 @@
     </row>
     <row r="65">
       <c r="A65" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B65" s="6">
         <v>0.0</v>
@@ -33481,7 +33478,7 @@
     </row>
     <row r="66">
       <c r="A66" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B66" s="6">
         <v>1.0</v>
@@ -33535,7 +33532,7 @@
     </row>
     <row r="67">
       <c r="A67" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B67" s="6">
         <v>1.0</v>
@@ -33589,7 +33586,7 @@
     </row>
     <row r="68">
       <c r="A68" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B68" s="6">
         <v>0.0</v>
@@ -33643,7 +33640,7 @@
     </row>
     <row r="69">
       <c r="A69" s="9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B69" s="6">
         <v>0.0</v>
@@ -33697,7 +33694,7 @@
     </row>
     <row r="70">
       <c r="A70" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B70" s="6">
         <v>0.0</v>
@@ -33751,7 +33748,7 @@
     </row>
     <row r="71">
       <c r="A71" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B71" s="6">
         <v>1.0</v>
@@ -33805,7 +33802,7 @@
     </row>
     <row r="72">
       <c r="A72" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B72" s="10">
         <v>0.0</v>
@@ -33859,7 +33856,7 @@
     </row>
     <row r="73">
       <c r="A73" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B73" s="10">
         <v>1.0</v>
@@ -33913,7 +33910,7 @@
     </row>
     <row r="74">
       <c r="A74" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B74" s="10">
         <v>1.0</v>
@@ -33967,7 +33964,7 @@
     </row>
     <row r="75">
       <c r="A75" s="9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B75" s="10">
         <v>1.0</v>
@@ -34021,7 +34018,7 @@
     </row>
     <row r="76">
       <c r="A76" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B76" s="10">
         <v>0.0</v>
@@ -34075,7 +34072,7 @@
     </row>
     <row r="77">
       <c r="A77" s="9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B77" s="11">
         <v>0.0</v>
@@ -34129,7 +34126,7 @@
     </row>
     <row r="78">
       <c r="A78" s="9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B78" s="11">
         <v>0.0</v>
@@ -34183,7 +34180,7 @@
     </row>
     <row r="79">
       <c r="A79" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B79" s="11">
         <v>1.0</v>
@@ -34237,7 +34234,7 @@
     </row>
     <row r="80">
       <c r="A80" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B80" s="11">
         <v>0.0</v>
@@ -34291,7 +34288,7 @@
     </row>
     <row r="81">
       <c r="A81" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B81" s="11">
         <v>1.0</v>
@@ -34345,7 +34342,7 @@
     </row>
     <row r="82">
       <c r="A82" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B82" s="11">
         <v>1.0</v>
@@ -34399,7 +34396,7 @@
     </row>
     <row r="83">
       <c r="A83" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B83" s="11">
         <v>1.0</v>
@@ -34453,7 +34450,7 @@
     </row>
     <row r="84">
       <c r="A84" s="9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B84" s="11">
         <v>0.0</v>
@@ -34507,7 +34504,7 @@
     </row>
     <row r="85">
       <c r="A85" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B85" s="11">
         <v>0.0</v>
@@ -34561,7 +34558,7 @@
     </row>
     <row r="86">
       <c r="A86" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B86" s="11">
         <v>1.0</v>
@@ -34615,7 +34612,7 @@
     </row>
     <row r="87">
       <c r="A87" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B87" s="15">
         <v>1.0</v>
@@ -34669,7 +34666,7 @@
     </row>
     <row r="88">
       <c r="A88" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B88" s="15">
         <v>0.0</v>
@@ -34723,7 +34720,7 @@
     </row>
     <row r="89">
       <c r="A89" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B89" s="15">
         <v>0.0</v>
@@ -34777,7 +34774,7 @@
     </row>
     <row r="90">
       <c r="A90" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B90" s="15">
         <v>0.0</v>
@@ -34831,7 +34828,7 @@
     </row>
     <row r="91">
       <c r="A91" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B91" s="15">
         <v>0.0</v>
@@ -34885,7 +34882,7 @@
     </row>
     <row r="92">
       <c r="A92" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B92" s="15">
         <v>1.0</v>
@@ -34939,7 +34936,7 @@
     </row>
     <row r="93">
       <c r="A93" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B93" s="15">
         <v>1.0</v>
@@ -34993,7 +34990,7 @@
     </row>
     <row r="94">
       <c r="A94" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B94" s="15">
         <v>0.0</v>
@@ -35047,7 +35044,7 @@
     </row>
     <row r="95">
       <c r="A95" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B95" s="15">
         <v>0.0</v>
@@ -35101,7 +35098,7 @@
     </row>
     <row r="96">
       <c r="A96" s="9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B96" s="15">
         <v>1.0</v>
@@ -35155,7 +35152,7 @@
     </row>
     <row r="97">
       <c r="A97" s="9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B97" s="15">
         <v>0.0</v>
@@ -35209,7 +35206,7 @@
     </row>
     <row r="98">
       <c r="A98" s="9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B98" s="15">
         <v>1.0</v>
@@ -35263,7 +35260,7 @@
     </row>
     <row r="99">
       <c r="A99" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B99" s="15">
         <v>0.0</v>
@@ -35317,7 +35314,7 @@
     </row>
     <row r="100">
       <c r="A100" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B100" s="15">
         <v>1.0</v>
@@ -35371,7 +35368,7 @@
     </row>
     <row r="101">
       <c r="A101" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B101" s="15">
         <v>1.0</v>
@@ -35425,7 +35422,7 @@
     </row>
     <row r="102">
       <c r="A102" s="9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B102" s="15">
         <v>0.0</v>
@@ -35479,7 +35476,7 @@
     </row>
     <row r="103">
       <c r="A103" s="9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B103" s="15">
         <v>0.0</v>
@@ -35533,7 +35530,7 @@
     </row>
     <row r="104">
       <c r="A104" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B104" s="15">
         <v>1.0</v>
@@ -35587,7 +35584,7 @@
     </row>
     <row r="105">
       <c r="A105" s="9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B105" s="15">
         <v>1.0</v>
@@ -35641,7 +35638,7 @@
     </row>
     <row r="106">
       <c r="A106" s="9" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B106" s="15">
         <v>0.0</v>
@@ -35695,7 +35692,7 @@
     </row>
     <row r="107">
       <c r="A107" s="9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B107" s="15">
         <v>0.0</v>
@@ -35749,7 +35746,7 @@
     </row>
     <row r="108">
       <c r="A108" s="9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B108" s="15">
         <v>1.0</v>
@@ -35803,7 +35800,7 @@
     </row>
     <row r="109">
       <c r="A109" s="9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B109" s="15">
         <v>1.0</v>
@@ -35857,7 +35854,7 @@
     </row>
     <row r="110">
       <c r="A110" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B110" s="15">
         <v>0.0</v>
@@ -35911,7 +35908,7 @@
     </row>
     <row r="111">
       <c r="A111" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B111" s="15">
         <v>1.0</v>
@@ -35965,7 +35962,7 @@
     </row>
     <row r="112">
       <c r="A112" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B112" s="15">
         <v>1.0</v>
@@ -36019,7 +36016,7 @@
     </row>
     <row r="113">
       <c r="A113" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B113" s="15">
         <v>1.0</v>
@@ -36073,7 +36070,7 @@
     </row>
     <row r="114">
       <c r="A114" s="9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B114" s="15">
         <v>0.0</v>
@@ -36127,7 +36124,7 @@
     </row>
     <row r="115">
       <c r="A115" s="9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B115" s="15">
         <v>1.0</v>
@@ -36181,7 +36178,7 @@
     </row>
     <row r="116">
       <c r="A116" s="9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B116" s="15">
         <v>1.0</v>
@@ -36235,7 +36232,7 @@
     </row>
     <row r="117">
       <c r="A117" s="9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B117" s="15">
         <v>0.0</v>
@@ -36289,7 +36286,7 @@
     </row>
     <row r="118">
       <c r="A118" s="9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B118" s="15">
         <v>0.0</v>
@@ -36343,7 +36340,7 @@
     </row>
     <row r="119">
       <c r="A119" s="9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B119" s="15">
         <v>0.0</v>
@@ -36397,7 +36394,7 @@
     </row>
     <row r="120">
       <c r="A120" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B120" s="15">
         <v>0.0</v>
@@ -36451,7 +36448,7 @@
     </row>
     <row r="121">
       <c r="A121" s="9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B121" s="15">
         <v>0.0</v>
@@ -36505,7 +36502,7 @@
     </row>
     <row r="122">
       <c r="A122" s="9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B122" s="15">
         <v>1.0</v>
@@ -36559,7 +36556,7 @@
     </row>
     <row r="123">
       <c r="A123" s="9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B123" s="15">
         <v>0.0</v>
@@ -36613,7 +36610,7 @@
     </row>
     <row r="124">
       <c r="A124" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B124" s="15">
         <v>1.0</v>
@@ -36667,7 +36664,7 @@
     </row>
     <row r="125">
       <c r="A125" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B125" s="15">
         <v>1.0</v>
@@ -36721,7 +36718,7 @@
     </row>
     <row r="126">
       <c r="A126" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B126" s="15">
         <v>0.0</v>
@@ -36775,7 +36772,7 @@
     </row>
     <row r="127">
       <c r="A127" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B127" s="15">
         <v>0.0</v>
@@ -36829,7 +36826,7 @@
     </row>
     <row r="128">
       <c r="A128" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B128" s="15">
         <v>0.0</v>
@@ -36883,7 +36880,7 @@
     </row>
     <row r="129">
       <c r="A129" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B129" s="15">
         <v>1.0</v>
@@ -36937,7 +36934,7 @@
     </row>
     <row r="130">
       <c r="A130" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B130" s="15">
         <v>1.0</v>
@@ -36991,7 +36988,7 @@
     </row>
     <row r="131">
       <c r="A131" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B131" s="15">
         <v>1.0</v>
@@ -37045,7 +37042,7 @@
     </row>
     <row r="132">
       <c r="A132" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B132" s="15">
         <v>0.0</v>
@@ -37099,7 +37096,7 @@
     </row>
     <row r="133">
       <c r="A133" s="9" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B133" s="15">
         <v>1.0</v>
@@ -37153,7 +37150,7 @@
     </row>
     <row r="134">
       <c r="A134" s="9" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B134" s="15">
         <v>1.0</v>
@@ -37207,7 +37204,7 @@
     </row>
     <row r="135">
       <c r="A135" s="9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B135" s="15">
         <v>0.0</v>
@@ -37261,7 +37258,7 @@
     </row>
     <row r="136">
       <c r="A136" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B136" s="15">
         <v>1.0</v>
@@ -37315,7 +37312,7 @@
     </row>
     <row r="137">
       <c r="A137" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B137" s="15">
         <v>0.0</v>
@@ -37369,7 +37366,7 @@
     </row>
     <row r="138">
       <c r="A138" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B138" s="15">
         <v>1.0</v>
@@ -37423,7 +37420,7 @@
     </row>
     <row r="139">
       <c r="A139" s="9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B139" s="15">
         <v>1.0</v>
@@ -37477,7 +37474,7 @@
     </row>
     <row r="140">
       <c r="A140" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B140" s="15">
         <v>0.0</v>
@@ -37531,7 +37528,7 @@
     </row>
     <row r="141">
       <c r="A141" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B141" s="15">
         <v>1.0</v>
@@ -37585,7 +37582,7 @@
     </row>
     <row r="142">
       <c r="A142" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B142" s="15">
         <v>1.0</v>
@@ -37639,7 +37636,7 @@
     </row>
     <row r="143">
       <c r="A143" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B143" s="15">
         <v>0.0</v>
@@ -37693,7 +37690,7 @@
     </row>
     <row r="144">
       <c r="A144" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B144" s="15">
         <v>0.0</v>
@@ -37747,7 +37744,7 @@
     </row>
     <row r="145">
       <c r="A145" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B145" s="15">
         <v>0.0</v>
@@ -37801,7 +37798,7 @@
     </row>
     <row r="146">
       <c r="A146" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B146" s="15">
         <v>0.0</v>
@@ -37855,7 +37852,7 @@
     </row>
     <row r="147">
       <c r="A147" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B147" s="15">
         <v>1.0</v>
@@ -37909,7 +37906,7 @@
     </row>
     <row r="148">
       <c r="A148" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B148" s="15">
         <v>0.0</v>
@@ -37963,7 +37960,7 @@
     </row>
     <row r="149">
       <c r="A149" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B149" s="15">
         <v>1.0</v>
@@ -38017,7 +38014,7 @@
     </row>
     <row r="150">
       <c r="A150" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B150" s="15">
         <v>0.0</v>
@@ -38071,7 +38068,7 @@
     </row>
     <row r="151">
       <c r="A151" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B151" s="15">
         <v>0.0</v>
@@ -38125,7 +38122,7 @@
     </row>
     <row r="152">
       <c r="A152" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B152" s="15">
         <v>1.0</v>
@@ -38179,7 +38176,7 @@
     </row>
     <row r="153">
       <c r="A153" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B153" s="15">
         <v>1.0</v>
@@ -38233,7 +38230,7 @@
     </row>
     <row r="154">
       <c r="A154" s="9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B154" s="15">
         <v>0.0</v>
@@ -38287,7 +38284,7 @@
     </row>
     <row r="155">
       <c r="A155" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B155" s="15">
         <v>1.0</v>
@@ -38341,7 +38338,7 @@
     </row>
     <row r="156">
       <c r="A156" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B156" s="15">
         <v>0.0</v>
@@ -38395,7 +38392,7 @@
     </row>
     <row r="157">
       <c r="A157" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B157" s="15">
         <v>0.0</v>
@@ -38449,7 +38446,7 @@
     </row>
     <row r="158">
       <c r="A158" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B158" s="15">
         <v>0.0</v>
@@ -38503,7 +38500,7 @@
     </row>
     <row r="159">
       <c r="A159" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B159" s="15">
         <v>1.0</v>
@@ -38557,7 +38554,7 @@
     </row>
     <row r="160">
       <c r="A160" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B160" s="15">
         <v>1.0</v>
@@ -38611,7 +38608,7 @@
     </row>
     <row r="161">
       <c r="A161" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B161" s="15">
         <v>0.0</v>
@@ -38665,7 +38662,7 @@
     </row>
     <row r="162">
       <c r="A162" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B162" s="15">
         <v>1.0</v>
@@ -38719,7 +38716,7 @@
     </row>
     <row r="163">
       <c r="A163" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B163" s="15">
         <v>0.0</v>
@@ -38773,7 +38770,7 @@
     </row>
     <row r="164">
       <c r="A164" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B164" s="15">
         <v>1.0</v>
@@ -38827,7 +38824,7 @@
     </row>
     <row r="165">
       <c r="A165" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B165" s="15">
         <v>1.0</v>
@@ -38881,7 +38878,7 @@
     </row>
     <row r="166">
       <c r="A166" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B166" s="15">
         <v>0.0</v>
@@ -38935,7 +38932,7 @@
     </row>
     <row r="167">
       <c r="A167" s="9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B167" s="15">
         <v>1.0</v>
@@ -38989,7 +38986,7 @@
     </row>
     <row r="168">
       <c r="A168" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B168" s="15">
         <v>1.0</v>
@@ -39043,7 +39040,7 @@
     </row>
     <row r="169">
       <c r="A169" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B169" s="15">
         <v>1.0</v>
@@ -39097,7 +39094,7 @@
     </row>
     <row r="170">
       <c r="A170" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B170" s="15">
         <v>0.0</v>
@@ -39151,7 +39148,7 @@
     </row>
     <row r="171">
       <c r="A171" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B171" s="15">
         <v>0.0</v>
@@ -39205,7 +39202,7 @@
     </row>
     <row r="172">
       <c r="A172" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B172" s="15">
         <v>0.0</v>
@@ -39259,7 +39256,7 @@
     </row>
     <row r="173">
       <c r="A173" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B173" s="15">
         <v>0.0</v>
@@ -39313,7 +39310,7 @@
     </row>
     <row r="174">
       <c r="A174" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B174" s="15">
         <v>1.0</v>
@@ -39367,7 +39364,7 @@
     </row>
     <row r="175">
       <c r="A175" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B175" s="15">
         <v>1.0</v>
@@ -39421,7 +39418,7 @@
     </row>
     <row r="176">
       <c r="A176" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B176" s="15">
         <v>1.0</v>
@@ -39475,7 +39472,7 @@
     </row>
     <row r="177">
       <c r="A177" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B177" s="15">
         <v>0.0</v>
@@ -39529,7 +39526,7 @@
     </row>
     <row r="178">
       <c r="A178" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B178" s="15">
         <v>0.0</v>
@@ -39583,7 +39580,7 @@
     </row>
     <row r="179">
       <c r="A179" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B179" s="15">
         <v>0.0</v>
@@ -39637,7 +39634,7 @@
     </row>
     <row r="180">
       <c r="A180" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B180" s="15">
         <v>1.0</v>
@@ -39691,7 +39688,7 @@
     </row>
     <row r="181">
       <c r="A181" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B181" s="15">
         <v>1.0</v>
@@ -39745,7 +39742,7 @@
     </row>
     <row r="182">
       <c r="A182" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B182" s="15">
         <v>0.0</v>
@@ -39799,7 +39796,7 @@
     </row>
     <row r="183">
       <c r="A183" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B183" s="15">
         <v>0.0</v>
@@ -39853,7 +39850,7 @@
     </row>
     <row r="184">
       <c r="A184" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B184" s="15">
         <v>0.0</v>
@@ -39907,7 +39904,7 @@
     </row>
     <row r="185">
       <c r="A185" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B185" s="15">
         <v>0.0</v>
@@ -39961,7 +39958,7 @@
     </row>
     <row r="186">
       <c r="A186" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B186" s="15">
         <v>1.0</v>
@@ -40015,7 +40012,7 @@
     </row>
     <row r="187">
       <c r="A187" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B187" s="15">
         <v>1.0</v>
@@ -40069,7 +40066,7 @@
     </row>
     <row r="188">
       <c r="A188" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B188" s="15">
         <v>0.0</v>
@@ -40123,7 +40120,7 @@
     </row>
     <row r="189">
       <c r="A189" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B189" s="15">
         <v>0.0</v>
@@ -40177,7 +40174,7 @@
     </row>
     <row r="190">
       <c r="A190" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B190" s="15">
         <v>0.0</v>
@@ -40231,7 +40228,7 @@
     </row>
     <row r="191">
       <c r="A191" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B191" s="15">
         <v>0.0</v>
@@ -40285,7 +40282,7 @@
     </row>
     <row r="192">
       <c r="A192" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B192" s="15">
         <v>0.0</v>
@@ -40339,7 +40336,7 @@
     </row>
     <row r="193">
       <c r="A193" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B193" s="15">
         <v>0.0</v>
@@ -40393,7 +40390,7 @@
     </row>
     <row r="194">
       <c r="A194" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B194" s="15">
         <v>1.0</v>
@@ -40447,7 +40444,7 @@
     </row>
     <row r="195">
       <c r="A195" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B195" s="15">
         <v>0.0</v>
@@ -40501,7 +40498,7 @@
     </row>
     <row r="196">
       <c r="A196" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B196" s="15">
         <v>1.0</v>
@@ -40555,7 +40552,7 @@
     </row>
     <row r="197">
       <c r="A197" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B197" s="15">
         <v>0.0</v>
@@ -40609,7 +40606,7 @@
     </row>
     <row r="198">
       <c r="A198" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B198" s="15">
         <v>0.0</v>
@@ -40663,7 +40660,7 @@
     </row>
     <row r="199">
       <c r="A199" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B199" s="15">
         <v>0.0</v>
@@ -40717,7 +40714,7 @@
     </row>
     <row r="200">
       <c r="A200" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B200" s="15">
         <v>1.0</v>
@@ -40771,7 +40768,7 @@
     </row>
     <row r="201">
       <c r="A201" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B201" s="15">
         <v>0.0</v>
@@ -40825,7 +40822,7 @@
     </row>
     <row r="202">
       <c r="A202" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B202" s="15">
         <v>1.0</v>
@@ -40879,7 +40876,7 @@
     </row>
     <row r="203">
       <c r="A203" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B203" s="15">
         <v>0.0</v>
@@ -40933,7 +40930,7 @@
     </row>
     <row r="204">
       <c r="A204" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B204" s="15">
         <v>0.0</v>
@@ -40987,7 +40984,7 @@
     </row>
     <row r="205">
       <c r="A205" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B205" s="15">
         <v>0.0</v>
@@ -41041,7 +41038,7 @@
     </row>
     <row r="206">
       <c r="A206" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B206" s="15">
         <v>0.0</v>
@@ -41095,7 +41092,7 @@
     </row>
     <row r="207">
       <c r="A207" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B207" s="15">
         <v>1.0</v>
@@ -41149,7 +41146,7 @@
     </row>
     <row r="208">
       <c r="A208" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B208" s="15">
         <v>1.0</v>
@@ -41203,7 +41200,7 @@
     </row>
     <row r="209">
       <c r="A209" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B209" s="15">
         <v>1.0</v>
@@ -41257,7 +41254,7 @@
     </row>
     <row r="210">
       <c r="A210" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B210" s="15">
         <v>1.0</v>
@@ -41311,7 +41308,7 @@
     </row>
     <row r="211">
       <c r="A211" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B211" s="15">
         <v>1.0</v>
@@ -41365,7 +41362,7 @@
     </row>
     <row r="212">
       <c r="A212" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B212" s="15">
         <v>0.0</v>
@@ -41419,7 +41416,7 @@
     </row>
     <row r="213">
       <c r="A213" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B213" s="15">
         <v>0.0</v>
@@ -41473,7 +41470,7 @@
     </row>
     <row r="214">
       <c r="A214" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B214" s="15">
         <v>1.0</v>
@@ -41527,7 +41524,7 @@
     </row>
     <row r="215">
       <c r="A215" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B215" s="15">
         <v>0.0</v>
@@ -41581,7 +41578,7 @@
     </row>
     <row r="216">
       <c r="A216" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B216" s="15">
         <v>0.0</v>
@@ -41635,7 +41632,7 @@
     </row>
     <row r="217">
       <c r="A217" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B217" s="15">
         <v>0.0</v>
@@ -41689,7 +41686,7 @@
     </row>
     <row r="218">
       <c r="A218" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B218" s="15">
         <v>0.0</v>
@@ -41743,7 +41740,7 @@
     </row>
     <row r="219">
       <c r="A219" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B219" s="15">
         <v>1.0</v>
@@ -41797,7 +41794,7 @@
     </row>
     <row r="220">
       <c r="A220" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B220" s="15">
         <v>1.0</v>
@@ -41851,7 +41848,7 @@
     </row>
     <row r="221">
       <c r="A221" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B221" s="15">
         <v>1.0</v>
@@ -41905,7 +41902,7 @@
     </row>
     <row r="222">
       <c r="A222" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B222" s="15">
         <v>0.0</v>
@@ -41959,7 +41956,7 @@
     </row>
     <row r="223">
       <c r="A223" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B223" s="15">
         <v>0.0</v>
@@ -42013,7 +42010,7 @@
     </row>
     <row r="224">
       <c r="A224" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B224" s="15">
         <v>0.0</v>
@@ -42067,7 +42064,7 @@
     </row>
     <row r="225">
       <c r="A225" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B225" s="15">
         <v>0.0</v>
@@ -42121,7 +42118,7 @@
     </row>
     <row r="226">
       <c r="A226" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B226" s="15">
         <v>0.0</v>
@@ -42175,7 +42172,7 @@
     </row>
     <row r="227">
       <c r="A227" s="9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B227" s="10">
         <v>0.0</v>
@@ -42229,7 +42226,7 @@
     </row>
     <row r="228">
       <c r="A228" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B228" s="10">
         <v>1.0</v>
@@ -42283,7 +42280,7 @@
     </row>
     <row r="229">
       <c r="A229" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B229" s="10">
         <v>1.0</v>
@@ -42337,7 +42334,7 @@
     </row>
     <row r="230">
       <c r="A230" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B230" s="10">
         <v>1.0</v>
@@ -57090,7 +57087,7 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B2" s="17">
         <v>0.0</v>
@@ -57143,7 +57140,7 @@
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B3" s="17">
         <v>0.0</v>
@@ -57196,7 +57193,7 @@
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B4" s="17">
         <v>0.0</v>
@@ -57249,18 +57246,20 @@
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="B5" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>509</v>
       </c>
-      <c r="B5" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="C5" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="19"/>
       <c r="F5" s="17">
         <v>0.0</v>
       </c>
@@ -57417,7 +57416,9 @@
       <c r="D8" s="17">
         <v>1.0</v>
       </c>
-      <c r="E8" s="19"/>
+      <c r="E8" s="18" t="s">
+        <v>509</v>
+      </c>
       <c r="F8" s="17">
         <v>0.0</v>
       </c>
@@ -57468,7 +57469,9 @@
       <c r="D9" s="17">
         <v>1.0</v>
       </c>
-      <c r="E9" s="19"/>
+      <c r="E9" s="18" t="s">
+        <v>509</v>
+      </c>
       <c r="F9" s="17">
         <v>0.0</v>
       </c>
@@ -57519,7 +57522,9 @@
       <c r="D10" s="17">
         <v>1.0</v>
       </c>
-      <c r="E10" s="19"/>
+      <c r="E10" s="18" t="s">
+        <v>509</v>
+      </c>
       <c r="F10" s="17">
         <v>0.0</v>
       </c>

</xml_diff>